<commit_message>
DMR_Parser v2.4: Fixed error that occured when combining the effluent data table with the effluent limit table; Added additional parameter code for Chloride to parameters table
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhudson\Documents\R Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lhudson\Documents\aquaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25706EB-33DB-4621-8725-B5205447B1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE94D5A2-DC7E-45C1-B6B6-4B140D405F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="600" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>parameter_code</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>74076</t>
+  </si>
+  <si>
+    <t>00940</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,14 +688,14 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>70295</v>
+      <c r="A14" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
@@ -700,24 +703,24 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
+        <v>70295</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>71850</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -728,13 +731,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>43</v>
@@ -742,15 +745,29 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>